<commit_message>
DWNSMP LBL files 50%
</commit_message>
<xml_diff>
--- a/To-Do list.xlsx
+++ b/To-Do list.xlsx
@@ -10,7 +10,7 @@
     <sheet name="To-do list" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To-do list'!$B$4:$B$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'To-do list'!$B$4:$B$28</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -42,19 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Geneva"/>
-          </rPr>
-          <t>To add more lines, press Tab in the last row of the table.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F25" authorId="0">
+    <comment ref="F21" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,12 +65,24 @@
         </r>
       </text>
     </comment>
+    <comment ref="F42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Geneva"/>
+          </rPr>
+          <t>To add more lines, press Tab in the last row of the table.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Done?</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>ta bort alla värden på första potentialen</t>
+  </si>
+  <si>
+    <t>LBL Files</t>
+  </si>
+  <si>
+    <t>First archive</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Blocklist</t>
+  </si>
+  <si>
+    <t>DWNSMPL</t>
+  </si>
+  <si>
+    <t>working</t>
+  </si>
+  <si>
+    <t>phys parameters</t>
+  </si>
+  <si>
+    <t>50%, ska implementeras överallt</t>
+  </si>
+  <si>
+    <t>send to Imperial College London after completion</t>
   </si>
 </sst>
 </file>
@@ -181,10 +208,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -407,92 +442,102 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -502,6 +547,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -511,9 +558,178 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="31">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color indexed="9"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="54"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1072,43 +1288,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E13" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:E13" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="B4:E13"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Done?" dataDxfId="19"/>
-    <tableColumn id="2" name="LAPDOG" dataDxfId="18"/>
-    <tableColumn id="3" name="Datum" dataDxfId="17"/>
-    <tableColumn id="4" name="Notes" dataDxfId="16"/>
+    <tableColumn id="1" name="Done?" dataDxfId="27"/>
+    <tableColumn id="2" name="LAPDOG" dataDxfId="26"/>
+    <tableColumn id="3" name="Datum" dataDxfId="25"/>
+    <tableColumn id="4" name="Notes" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B16:F22" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="B16:F22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B16:F18" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="B16:F18"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done?" dataDxfId="12"/>
-    <tableColumn id="2" name="GITHUB" dataDxfId="11"/>
-    <tableColumn id="3" name="Due By" dataDxfId="10"/>
-    <tableColumn id="4" name="Notes" dataDxfId="9"/>
-    <tableColumn id="5" name="Notes2" dataDxfId="8"/>
+    <tableColumn id="1" name="Done?" dataDxfId="20"/>
+    <tableColumn id="2" name="GITHUB" dataDxfId="19"/>
+    <tableColumn id="3" name="Due By" dataDxfId="18"/>
+    <tableColumn id="4" name="Notes" dataDxfId="17"/>
+    <tableColumn id="5" name="Notes2" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="B25:F34" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="B25:F34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table225" displayName="Table225" ref="B21:F30" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="B21:F30"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Done?" dataDxfId="4"/>
-    <tableColumn id="2" name="LAPDOG ANALYS" dataDxfId="3"/>
-    <tableColumn id="3" name="Due By" dataDxfId="2"/>
-    <tableColumn id="4" name="Notes" dataDxfId="1"/>
-    <tableColumn id="5" name="Notes2" dataDxfId="0"/>
+    <tableColumn id="1" name="Done?" dataDxfId="12"/>
+    <tableColumn id="2" name="LAPDOG ANALYS" dataDxfId="11"/>
+    <tableColumn id="3" name="Due By" dataDxfId="10"/>
+    <tableColumn id="4" name="Notes" dataDxfId="9"/>
+    <tableColumn id="5" name="Notes2" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table224" displayName="Table224" ref="B36:F42" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="B36:F42"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Done?" dataDxfId="7"/>
+    <tableColumn id="2" name="LBL Files" dataDxfId="6"/>
+    <tableColumn id="3" name="Due By" dataDxfId="5"/>
+    <tableColumn id="4" name="Notes" dataDxfId="4"/>
+    <tableColumn id="5" name="Notes2" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1402,10 +1632,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B1:G34"/>
+  <dimension ref="B1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1423,10 +1653,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="55" customHeight="1">
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="22"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
@@ -1438,7 +1668,7 @@
       <c r="D2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="21">
         <v>41662</v>
       </c>
     </row>
@@ -1505,7 +1735,9 @@
         <v>15</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="F8" s="13"/>
     </row>
     <row r="9" spans="2:7">
@@ -1602,108 +1834,108 @@
         <v>25</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="F18" s="15"/>
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B19" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="15"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B20" s="2"/>
+      <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
       <c r="E20" s="5"/>
-      <c r="F20" s="15"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B21" s="2"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="15"/>
+      <c r="B21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>20</v>
+      </c>
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B22" s="2"/>
-      <c r="C22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="5"/>
-      <c r="F22" s="16"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="2:7" s="3" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B24" s="4"/>
-      <c r="C24" s="5"/>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>3</v>
+      </c>
       <c r="D24" s="6"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B25" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B26" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="6"/>
       <c r="E26" s="5"/>
       <c r="F26" s="18"/>
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="6"/>
       <c r="E27" s="5"/>
       <c r="F27" s="18"/>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="5"/>
       <c r="D28" s="6"/>
       <c r="E28" s="5"/>
       <c r="F28" s="18"/>
@@ -1722,46 +1954,133 @@
       <c r="C30" s="5"/>
       <c r="D30" s="6"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="18"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="18"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="2:7" ht="16.5" customHeight="1">
-      <c r="B32" s="2"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="18"/>
       <c r="G32" s="5"/>
     </row>
-    <row r="33" spans="2:6">
-      <c r="B33" s="2"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" spans="2:6">
-      <c r="B34" s="2"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="19"/>
+    <row r="35" spans="2:7">
+      <c r="B35" s="7"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="15"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="15"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="8"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="2"/>
+      <c r="C40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="25">
+        <v>0</v>
+      </c>
+      <c r="F40" s="15"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="2"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="2"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="7"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="G45" s="5"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="G47" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="4">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="TODAY()-7"/>
@@ -1769,7 +2088,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:D34">
+  <conditionalFormatting sqref="D22:D30">
+    <cfRule type="iconSet" priority="2">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="formula" val="TODAY()-7"/>
+        <cfvo type="formula" val="TODAY()"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:D42">
     <cfRule type="iconSet" priority="1">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -1778,8 +2106,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:D22">
-    <cfRule type="iconSet" priority="4">
+  <conditionalFormatting sqref="D17:D18">
+    <cfRule type="iconSet" priority="6">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="TODAY()-7"/>
@@ -1788,7 +2116,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13 B26:B34 B17:B22">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B13 B22:B30 B17:B18 B37:B42">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1796,10 +2124,11 @@
   <pageMargins left="0.5" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
analysis 2.2 & LDLsweepcorrection
added 5 new variables, changed names on 2 variables
smoothening logic added
added kernels and updated metakernal_rosetta.txt (but these extra
kernels generates lots of errors after a few runs…?)
</commit_message>
<xml_diff>
--- a/To-Do list.xlsx
+++ b/To-Do list.xlsx
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>Done?</t>
   </si>
@@ -220,6 +220,24 @@
   </si>
   <si>
     <t>kan noteras</t>
+  </si>
+  <si>
+    <t>hysterisis på prob 2</t>
+  </si>
+  <si>
+    <t>Problem i alla svep</t>
+  </si>
+  <si>
+    <t>find Vbias (I2L), calculate hysteris according to simple model (linear from Email from Fredrik or other function by Anders)</t>
+  </si>
+  <si>
+    <t>lap_import</t>
+  </si>
+  <si>
+    <t>olsson analys modell?</t>
+  </si>
+  <si>
+    <t>olsson modell anpassning?</t>
   </si>
 </sst>
 </file>
@@ -229,10 +247,17 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -344,7 +369,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -469,114 +494,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="6" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -592,6 +663,7 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -607,6 +679,7 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
@@ -1348,8 +1421,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B21:F23" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
-  <autoFilter ref="B21:F23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table22" displayName="Table22" ref="B21:F24" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22" tableBorderDxfId="21">
+  <autoFilter ref="B21:F24"/>
   <tableColumns count="5">
     <tableColumn id="1" name="Done?" dataDxfId="20"/>
     <tableColumn id="2" name="GITHUB" dataDxfId="19"/>
@@ -1681,8 +1754,8 @@
   </sheetPr>
   <dimension ref="B1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1700,10 +1773,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="55" customHeight="1">
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1829,7 +1902,7 @@
       <c r="E12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="24" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1857,16 +1930,22 @@
       <c r="E14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="24" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="2:6" s="3" customFormat="1" ht="16.5" customHeight="1">
       <c r="B15" s="4"/>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="14"/>
+      <c r="E15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="2:6" ht="16.5" customHeight="1"/>
     <row r="17" spans="2:8" ht="16.5" customHeight="1"/>
@@ -1927,11 +2006,17 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
+      <c r="B24" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="31"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="2:8" ht="16.5" customHeight="1">
@@ -1997,7 +2082,9 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="2:8" ht="16.5" customHeight="1">
-      <c r="B30" s="2"/>
+      <c r="B30" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>44</v>
       </c>
@@ -2010,9 +2097,13 @@
     </row>
     <row r="31" spans="2:8" ht="16.5" customHeight="1">
       <c r="B31" s="2"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="D31" s="6"/>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="F31" s="18"/>
       <c r="G31" s="5"/>
     </row>
@@ -2163,9 +2254,9 @@
   <mergeCells count="1">
     <mergeCell ref="B1:C1"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="D5:D13">
-    <cfRule type="iconSet" priority="5">
+    <cfRule type="iconSet" priority="6">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="formula" val="TODAY()-7"/>
@@ -2174,6 +2265,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D35">
+    <cfRule type="iconSet" priority="4">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="formula" val="TODAY()-7"/>
+        <cfvo type="formula" val="TODAY()"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D42:D47">
     <cfRule type="iconSet" priority="3">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -2182,7 +2282,16 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42:D47">
+  <conditionalFormatting sqref="D22:D24">
+    <cfRule type="iconSet" priority="8">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="formula" val="TODAY()-7"/>
+        <cfvo type="formula" val="TODAY()"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D15">
     <cfRule type="iconSet" priority="2">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -2191,16 +2300,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D23">
-    <cfRule type="iconSet" priority="7">
-      <iconSet>
-        <cfvo type="percent" val="0"/>
-        <cfvo type="formula" val="TODAY()-7"/>
-        <cfvo type="formula" val="TODAY()"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D15">
+  <conditionalFormatting sqref="D24">
     <cfRule type="iconSet" priority="1">
       <iconSet>
         <cfvo type="percent" val="0"/>
@@ -2210,7 +2310,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B47 B27:B35 B22:B23 B5:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42:B47 B27:B35 B22:B24 B5:B15">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>